<commit_message>
Routin UC, add reserve constraints
</commit_message>
<xml_diff>
--- a/ams/cases/ieee39/ieee39_uced.xlsx
+++ b/ams/cases/ieee39/ieee39_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F76454-F4CC-0744-BD16-7A5A40DBC594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC80C5-94E8-1449-BFFC-3C65D8DEF3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="7420" windowWidth="21600" windowHeight="18940" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="14" r:id="rId1"/>
@@ -2986,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555DA4DC-13F2-134F-B8B2-A92CD209E2B3}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3026,7 +3026,7 @@
         <v>373</v>
       </c>
       <c r="E2" s="8">
-        <v>0.1</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>265</v>
@@ -3046,7 +3046,7 @@
         <v>374</v>
       </c>
       <c r="E3" s="8">
-        <v>0.1</v>
+        <v>2.46</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>266</v>
@@ -3066,7 +3066,7 @@
         <v>375</v>
       </c>
       <c r="E4" s="8">
-        <v>0.1</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>267</v>
@@ -3121,7 +3121,7 @@
         <v>376</v>
       </c>
       <c r="E2" s="8">
-        <v>0.1</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>265</v>
@@ -3141,7 +3141,7 @@
         <v>377</v>
       </c>
       <c r="E3" s="8">
-        <v>0.1</v>
+        <v>2.46</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>266</v>
@@ -3161,7 +3161,7 @@
         <v>378</v>
       </c>
       <c r="E4" s="8">
-        <v>0.1</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
Fix case ieee39_uced and ieee39_uced_vis
</commit_message>
<xml_diff>
--- a/ams/cases/ieee39/ieee39_uced.xlsx
+++ b/ams/cases/ieee39/ieee39_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320B54CF-92E6-1844-B920-D8352410805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EB796B-35CE-794D-9077-FB1B7B8BE12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="14" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="Region" sheetId="8" r:id="rId8"/>
     <sheet name="GCost" sheetId="6" r:id="rId9"/>
     <sheet name="EDTSlot" sheetId="12" r:id="rId10"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId11"/>
-    <sheet name="SFR" sheetId="9" r:id="rId12"/>
-    <sheet name="SFRCost" sheetId="10" r:id="rId13"/>
-    <sheet name="SR" sheetId="18" r:id="rId14"/>
-    <sheet name="SRCost" sheetId="20" r:id="rId15"/>
-    <sheet name="NSR" sheetId="19" r:id="rId16"/>
-    <sheet name="NSRCost" sheetId="21" r:id="rId17"/>
+    <sheet name="Shunt" sheetId="22" r:id="rId11"/>
+    <sheet name="UCTSlot" sheetId="13" r:id="rId12"/>
+    <sheet name="SFR" sheetId="9" r:id="rId13"/>
+    <sheet name="SFRCost" sheetId="10" r:id="rId14"/>
+    <sheet name="SR" sheetId="18" r:id="rId15"/>
+    <sheet name="SRCost" sheetId="20" r:id="rId16"/>
+    <sheet name="NSR" sheetId="19" r:id="rId17"/>
+    <sheet name="NSRCost" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="541">
   <si>
     <t>idx</t>
   </si>
@@ -1537,6 +1538,141 @@
   </si>
   <si>
     <t>1, 1, 1, 1, 1, 1, 1, 1, 1, 1</t>
+  </si>
+  <si>
+    <t>Shunt_1</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Shunt_2</t>
+  </si>
+  <si>
+    <t>1040</t>
+  </si>
+  <si>
+    <t>34.5</t>
+  </si>
+  <si>
+    <t>4.36086385</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.035534</t>
+  </si>
+  <si>
+    <t>836</t>
+  </si>
+  <si>
+    <t>6.45999998</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.013246</t>
+  </si>
+  <si>
+    <t>843.7</t>
+  </si>
+  <si>
+    <t>7.24999998</t>
+  </si>
+  <si>
+    <t>1.020528</t>
+  </si>
+  <si>
+    <t>1174.8</t>
+  </si>
+  <si>
+    <t>6.51999998</t>
+  </si>
+  <si>
+    <t>1.5806</t>
+  </si>
+  <si>
+    <t>1.01343</t>
+  </si>
+  <si>
+    <t>1080.2</t>
+  </si>
+  <si>
+    <t>15.5</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>1.5854</t>
+  </si>
+  <si>
+    <t>1.019109</t>
+  </si>
+  <si>
+    <t>1085.7</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>2.5777</t>
+  </si>
+  <si>
+    <t>1.06</t>
+  </si>
+  <si>
+    <t>1025.2</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>0.7876</t>
+  </si>
+  <si>
+    <t>970.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>1.013996</t>
+  </si>
+  <si>
+    <t>1684.1</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>1.428</t>
+  </si>
+  <si>
+    <t>1.052803</t>
+  </si>
+  <si>
+    <t>1199</t>
+  </si>
+  <si>
+    <t>5.7417</t>
+  </si>
+  <si>
+    <t>0.5617</t>
+  </si>
+  <si>
+    <t>1.03</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1678,6 +1814,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2051,7 +2190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E68EB-A0F6-9442-8602-C20717626DB0}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2493,6 +2632,117 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABE8D1C-05FB-B141-9D6A-355DC8C756E6}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>496</v>
+      </c>
+      <c r="E2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2" t="s">
+        <v>498</v>
+      </c>
+      <c r="H2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" t="s">
+        <v>500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" t="s">
+        <v>497</v>
+      </c>
+      <c r="G3" t="s">
+        <v>498</v>
+      </c>
+      <c r="H3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" t="s">
+        <v>189</v>
+      </c>
+      <c r="J3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -2862,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F77866-C777-0B41-8C14-27D8C9A5BF9B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2947,7 +3197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE302B1E-1C21-5545-8C07-A8652D0B6F47}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3183,7 +3433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F41B66-3F5A-A846-A642-21ADD81835C9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3259,7 +3509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F8382B-5372-9443-A9F0-6DD466EDEE98}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -3462,7 +3712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC710CCF-6BF4-8444-9442-818618AF42C4}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3538,7 +3788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9484A1E6-40ED-8148-BBE3-6D006206561E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -5406,7 +5656,7 @@
   <sheetViews>
     <sheetView zoomScale="159" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5466,7 +5716,7 @@
         <v>345</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="H2">
         <v>2.5</v>
@@ -5501,7 +5751,7 @@
         <v>345</v>
       </c>
       <c r="G3">
-        <v>4.5</v>
+        <v>3.6</v>
       </c>
       <c r="H3">
         <v>1.84</v>
@@ -5536,7 +5786,7 @@
         <v>345</v>
       </c>
       <c r="G4">
-        <v>2.3380000000000001</v>
+        <v>1.8704000000000001</v>
       </c>
       <c r="H4">
         <v>0.84</v>
@@ -5571,7 +5821,7 @@
         <v>345</v>
       </c>
       <c r="G5">
-        <v>5.22</v>
+        <v>4.1760000000000002</v>
       </c>
       <c r="H5">
         <v>1.766</v>
@@ -5606,7 +5856,7 @@
         <v>138</v>
       </c>
       <c r="G6">
-        <v>1.2</v>
+        <v>0.96</v>
       </c>
       <c r="H6">
         <v>0.3</v>
@@ -5641,7 +5891,7 @@
         <v>345</v>
       </c>
       <c r="G7">
-        <v>3.2</v>
+        <v>2.5600000000000005</v>
       </c>
       <c r="H7">
         <v>1.53</v>
@@ -5676,7 +5926,7 @@
         <v>345</v>
       </c>
       <c r="G8">
-        <v>3.29</v>
+        <v>2.6320000000000001</v>
       </c>
       <c r="H8">
         <v>0.32299999999999995</v>
@@ -5711,7 +5961,7 @@
         <v>345</v>
       </c>
       <c r="G9">
-        <v>1.58</v>
+        <v>1.2640000000000002</v>
       </c>
       <c r="H9">
         <v>0.3</v>
@@ -5746,7 +5996,7 @@
         <v>138</v>
       </c>
       <c r="G10">
-        <v>6.8</v>
+        <v>5.44</v>
       </c>
       <c r="H10">
         <v>1.03</v>
@@ -5781,7 +6031,7 @@
         <v>345</v>
       </c>
       <c r="G11">
-        <v>2.74</v>
+        <v>2.1920000000000002</v>
       </c>
       <c r="H11">
         <v>1.1499999999999999</v>
@@ -5816,7 +6066,7 @@
         <v>345</v>
       </c>
       <c r="G12">
-        <v>2.4750000000000001</v>
+        <v>1.9800000000000002</v>
       </c>
       <c r="H12">
         <v>0.84599999999999997</v>
@@ -5851,7 +6101,7 @@
         <v>345</v>
       </c>
       <c r="G13">
-        <v>3.0860000000000003</v>
+        <v>2.4688000000000003</v>
       </c>
       <c r="H13">
         <v>-0.92200000000000004</v>
@@ -5886,7 +6136,7 @@
         <v>345</v>
       </c>
       <c r="G14">
-        <v>2.2400000000000002</v>
+        <v>1.7920000000000003</v>
       </c>
       <c r="H14">
         <v>0.47200000000000003</v>
@@ -5921,7 +6171,7 @@
         <v>345</v>
       </c>
       <c r="G15">
-        <v>1.39</v>
+        <v>1.1119999999999999</v>
       </c>
       <c r="H15">
         <v>0.17</v>
@@ -5956,7 +6206,7 @@
         <v>345</v>
       </c>
       <c r="G16">
-        <v>2.81</v>
+        <v>2.2480000000000002</v>
       </c>
       <c r="H16">
         <v>0.755</v>
@@ -5991,7 +6241,7 @@
         <v>345</v>
       </c>
       <c r="G17">
-        <v>2.06</v>
+        <v>1.6480000000000001</v>
       </c>
       <c r="H17">
         <v>0.27600000000000002</v>
@@ -6026,7 +6276,7 @@
         <v>345</v>
       </c>
       <c r="G18">
-        <v>2.835</v>
+        <v>2.2680000000000002</v>
       </c>
       <c r="H18">
         <v>1.2690000000000001</v>
@@ -6061,7 +6311,7 @@
         <v>34.5</v>
       </c>
       <c r="G19">
-        <v>0.8</v>
+        <v>0.64000000000000012</v>
       </c>
       <c r="H19">
         <v>0.4</v>
@@ -6096,7 +6346,7 @@
         <v>345</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="H20">
         <v>2.5</v>
@@ -6120,9 +6370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6241,11 +6491,11 @@
       <c r="D2" t="s">
         <v>336</v>
       </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>345</v>
+      <c r="E2" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>502</v>
       </c>
       <c r="G2">
         <v>30</v>
@@ -6253,26 +6503,26 @@
       <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2">
-        <v>6.5</v>
-      </c>
-      <c r="J2">
-        <v>1.6176200000000001</v>
-      </c>
-      <c r="K2">
-        <v>10.4</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>4</v>
-      </c>
-      <c r="N2">
-        <v>1.4</v>
-      </c>
-      <c r="O2">
-        <v>1.0499000000000001</v>
+      <c r="I2" t="s">
+        <v>503</v>
+      </c>
+      <c r="J2" t="s">
+        <v>504</v>
+      </c>
+      <c r="K2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="2">
+        <v>99</v>
+      </c>
+      <c r="N2" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O2" t="s">
+        <v>505</v>
       </c>
       <c r="P2">
         <v>1.4</v>
@@ -6342,11 +6592,11 @@
       <c r="D3" t="s">
         <v>337</v>
       </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>345</v>
+      <c r="E3" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>502</v>
       </c>
       <c r="G3">
         <v>31</v>
@@ -6354,26 +6604,26 @@
       <c r="H3">
         <v>32</v>
       </c>
-      <c r="I3">
-        <v>6.5</v>
-      </c>
-      <c r="J3">
-        <v>2.0696500000000002</v>
-      </c>
-      <c r="K3">
-        <v>7.25</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>1.5</v>
-      </c>
-      <c r="O3">
-        <v>0.98409999999999997</v>
+      <c r="I3" t="s">
+        <v>507</v>
+      </c>
+      <c r="J3" t="s">
+        <v>190</v>
+      </c>
+      <c r="K3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L3" t="s">
+        <v>508</v>
+      </c>
+      <c r="M3" s="2">
+        <v>99</v>
+      </c>
+      <c r="N3" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>509</v>
       </c>
       <c r="P3">
         <v>1.4</v>
@@ -6443,11 +6693,11 @@
       <c r="D4" t="s">
         <v>338</v>
       </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>345</v>
+      <c r="E4" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="G4">
         <v>32</v>
@@ -6455,26 +6705,26 @@
       <c r="H4">
         <v>33</v>
       </c>
-      <c r="I4">
-        <v>6.5</v>
-      </c>
-      <c r="J4">
-        <v>1.0829299999999999</v>
-      </c>
-      <c r="K4">
-        <v>6.52</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>2.5</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0.99719999999999998</v>
+      <c r="I4" t="s">
+        <v>511</v>
+      </c>
+      <c r="J4" t="s">
+        <v>190</v>
+      </c>
+      <c r="K4" t="s">
+        <v>195</v>
+      </c>
+      <c r="L4" t="s">
+        <v>188</v>
+      </c>
+      <c r="M4" s="2">
+        <v>99</v>
+      </c>
+      <c r="N4" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O4" t="s">
+        <v>512</v>
       </c>
       <c r="P4">
         <v>1.4</v>
@@ -6544,11 +6794,11 @@
       <c r="D5" t="s">
         <v>339</v>
       </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>345</v>
+      <c r="E5" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="G5">
         <v>33</v>
@@ -6556,26 +6806,26 @@
       <c r="H5">
         <v>34</v>
       </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>1.6668799999999999</v>
-      </c>
-      <c r="K5">
-        <v>5.08</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>1.67</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>1.0123</v>
+      <c r="I5" t="s">
+        <v>514</v>
+      </c>
+      <c r="J5" t="s">
+        <v>515</v>
+      </c>
+      <c r="K5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" s="2">
+        <v>99</v>
+      </c>
+      <c r="N5" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O5" t="s">
+        <v>516</v>
       </c>
       <c r="P5">
         <v>1.4</v>
@@ -6645,11 +6895,11 @@
       <c r="D6" t="s">
         <v>340</v>
       </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>345</v>
+      <c r="E6" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>518</v>
       </c>
       <c r="G6">
         <v>34</v>
@@ -6657,26 +6907,26 @@
       <c r="H6">
         <v>35</v>
       </c>
-      <c r="I6">
-        <v>6.6</v>
-      </c>
-      <c r="J6">
-        <v>2.1066099999999999</v>
-      </c>
-      <c r="K6">
-        <v>6.87</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6">
-        <v>-1</v>
-      </c>
-      <c r="O6">
-        <v>1.0494000000000001</v>
+      <c r="I6" t="s">
+        <v>519</v>
+      </c>
+      <c r="J6" t="s">
+        <v>520</v>
+      </c>
+      <c r="K6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L6" t="s">
+        <v>188</v>
+      </c>
+      <c r="M6" s="2">
+        <v>99</v>
+      </c>
+      <c r="N6" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O6" t="s">
+        <v>521</v>
       </c>
       <c r="P6">
         <v>1.4</v>
@@ -6746,11 +6996,11 @@
       <c r="D7" t="s">
         <v>341</v>
       </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>345</v>
+      <c r="E7" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>518</v>
       </c>
       <c r="G7">
         <v>35</v>
@@ -6758,26 +7008,26 @@
       <c r="H7">
         <v>36</v>
       </c>
-      <c r="I7">
-        <v>5.6</v>
-      </c>
-      <c r="J7">
-        <v>1.0016499999999999</v>
-      </c>
-      <c r="K7">
-        <v>5.8</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>2.4</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1.0636000000000001</v>
+      <c r="I7" t="s">
+        <v>523</v>
+      </c>
+      <c r="J7" t="s">
+        <v>524</v>
+      </c>
+      <c r="K7" t="s">
+        <v>195</v>
+      </c>
+      <c r="L7" t="s">
+        <v>198</v>
+      </c>
+      <c r="M7" s="2">
+        <v>99</v>
+      </c>
+      <c r="N7" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O7" t="s">
+        <v>525</v>
       </c>
       <c r="P7">
         <v>1.4</v>
@@ -6847,11 +7097,11 @@
       <c r="D8" t="s">
         <v>342</v>
       </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>345</v>
+      <c r="E8" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>527</v>
       </c>
       <c r="G8">
         <v>36</v>
@@ -6859,26 +7109,26 @@
       <c r="H8">
         <v>37</v>
       </c>
-      <c r="I8">
-        <v>5.4</v>
-      </c>
-      <c r="J8">
-        <v>-1.36945E-2</v>
-      </c>
-      <c r="K8">
-        <v>5.64</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>2.5</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>1.0275000000000001</v>
+      <c r="I8" t="s">
+        <v>528</v>
+      </c>
+      <c r="J8" t="s">
+        <v>529</v>
+      </c>
+      <c r="K8" t="s">
+        <v>194</v>
+      </c>
+      <c r="L8" t="s">
+        <v>188</v>
+      </c>
+      <c r="M8" s="2">
+        <v>99</v>
+      </c>
+      <c r="N8" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O8" t="s">
+        <v>525</v>
       </c>
       <c r="P8">
         <v>1.4</v>
@@ -6948,11 +7198,11 @@
       <c r="D9" t="s">
         <v>343</v>
       </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9">
-        <v>345</v>
+      <c r="E9" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>527</v>
       </c>
       <c r="G9">
         <v>37</v>
@@ -6960,26 +7210,26 @@
       <c r="H9">
         <v>38</v>
       </c>
-      <c r="I9">
-        <v>6.5</v>
-      </c>
-      <c r="J9">
-        <v>0.21732699999999999</v>
-      </c>
-      <c r="K9">
-        <v>8.65</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
-        <v>-1.5</v>
-      </c>
-      <c r="O9">
-        <v>1.0265</v>
+      <c r="I9" t="s">
+        <v>531</v>
+      </c>
+      <c r="J9" t="s">
+        <v>198</v>
+      </c>
+      <c r="K9" t="s">
+        <v>194</v>
+      </c>
+      <c r="L9" t="s">
+        <v>198</v>
+      </c>
+      <c r="M9" s="2">
+        <v>99</v>
+      </c>
+      <c r="N9" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O9" t="s">
+        <v>532</v>
       </c>
       <c r="P9">
         <v>1.4</v>
@@ -7049,11 +7299,11 @@
       <c r="D10" t="s">
         <v>344</v>
       </c>
-      <c r="E10">
-        <v>100</v>
-      </c>
-      <c r="F10">
-        <v>345</v>
+      <c r="E10" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>502</v>
       </c>
       <c r="G10">
         <v>38</v>
@@ -7061,26 +7311,26 @@
       <c r="H10">
         <v>39</v>
       </c>
-      <c r="I10">
-        <v>6.5</v>
-      </c>
-      <c r="J10">
-        <v>0.78467399999999998</v>
-      </c>
-      <c r="K10">
-        <v>11</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>-1</v>
-      </c>
-      <c r="O10">
-        <v>1.03</v>
+      <c r="I10" t="s">
+        <v>534</v>
+      </c>
+      <c r="J10" t="s">
+        <v>535</v>
+      </c>
+      <c r="K10" t="s">
+        <v>197</v>
+      </c>
+      <c r="L10" t="s">
+        <v>198</v>
+      </c>
+      <c r="M10" s="2">
+        <v>99</v>
+      </c>
+      <c r="N10" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O10" t="s">
+        <v>536</v>
       </c>
       <c r="P10">
         <v>1.4</v>
@@ -7149,7 +7399,7 @@
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7271,8 +7521,8 @@
       <c r="D2" t="s">
         <v>345</v>
       </c>
-      <c r="E2">
-        <v>100</v>
+      <c r="E2" s="12" t="s">
+        <v>537</v>
       </c>
       <c r="F2">
         <v>345</v>
@@ -7280,26 +7530,26 @@
       <c r="G2">
         <v>39</v>
       </c>
-      <c r="I2">
-        <v>6.7787100000000002</v>
-      </c>
-      <c r="J2">
-        <v>2.2157399999999998</v>
-      </c>
-      <c r="K2">
-        <v>15</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
-        <v>-1</v>
-      </c>
-      <c r="O2">
-        <v>0.98199999999999998</v>
+      <c r="I2" t="s">
+        <v>538</v>
+      </c>
+      <c r="J2" t="s">
+        <v>539</v>
+      </c>
+      <c r="K2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L2" t="s">
+        <v>190</v>
+      </c>
+      <c r="M2" s="2">
+        <v>99</v>
+      </c>
+      <c r="N2" s="2">
+        <v>-99</v>
+      </c>
+      <c r="O2" t="s">
+        <v>540</v>
       </c>
       <c r="P2">
         <v>1.4</v>
@@ -7370,7 +7620,7 @@
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>